<commit_message>
Prototype UWP app (not functional)
</commit_message>
<xml_diff>
--- a/SpeechMaps.xlsx
+++ b/SpeechMaps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Drohne\OpenTx\speechGenerator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Projects\Drone\Voice creater\OpenTx-googleTTS-soundpack-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5B2A6A-EB1C-4483-AFDE-55EB3735C499}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B091F99-CB3C-4363-BFF3-9277D2068C8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{6E96A293-20C0-483B-9069-E42BF2A79F63}"/>
+    <workbookView xWindow="-10530" yWindow="5130" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{6E96A293-20C0-483B-9069-E42BF2A79F63}"/>
   </bookViews>
   <sheets>
     <sheet name="de-DE-system" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2980" uniqueCount="1005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3019" uniqueCount="1044">
   <si>
     <t>Filename</t>
   </si>
@@ -3051,6 +3051,123 @@
   </si>
   <si>
     <t>m11</t>
+  </si>
+  <si>
+    <t>arm</t>
+  </si>
+  <si>
+    <t>Arm motors</t>
+  </si>
+  <si>
+    <t>Motors armed</t>
+  </si>
+  <si>
+    <t>bclow</t>
+  </si>
+  <si>
+    <t>Remaining battery capacity low</t>
+  </si>
+  <si>
+    <t>bproff</t>
+  </si>
+  <si>
+    <t>Beeper off</t>
+  </si>
+  <si>
+    <t>bpron</t>
+  </si>
+  <si>
+    <t>Beeper on</t>
+  </si>
+  <si>
+    <t>disarm</t>
+  </si>
+  <si>
+    <t>Motors disarmed</t>
+  </si>
+  <si>
+    <t>fmacro</t>
+  </si>
+  <si>
+    <t>Acro mode</t>
+  </si>
+  <si>
+    <t>fmgpsh</t>
+  </si>
+  <si>
+    <t>GPS hold</t>
+  </si>
+  <si>
+    <t>fmrth</t>
+  </si>
+  <si>
+    <t>Return to home</t>
+  </si>
+  <si>
+    <t>fmstbl</t>
+  </si>
+  <si>
+    <t>Stabilized mode</t>
+  </si>
+  <si>
+    <t>gpsko</t>
+  </si>
+  <si>
+    <t>GPS lost</t>
+  </si>
+  <si>
+    <t>gpsok</t>
+  </si>
+  <si>
+    <t>GPS lock established</t>
+  </si>
+  <si>
+    <t>lqcrit</t>
+  </si>
+  <si>
+    <t>lqlow</t>
+  </si>
+  <si>
+    <t>Link quality low</t>
+  </si>
+  <si>
+    <t>Link quality critical</t>
+  </si>
+  <si>
+    <t>trtmoff</t>
+  </si>
+  <si>
+    <t>trtmon</t>
+  </si>
+  <si>
+    <t>Turtle mode off</t>
+  </si>
+  <si>
+    <t>Turtle mode on</t>
+  </si>
+  <si>
+    <t>urfast</t>
+  </si>
+  <si>
+    <t>urnorm</t>
+  </si>
+  <si>
+    <t>urslow</t>
+  </si>
+  <si>
+    <t>fmhl</t>
+  </si>
+  <si>
+    <t>Headless mode</t>
+  </si>
+  <si>
+    <t>Switched to 150Hz mode</t>
+  </si>
+  <si>
+    <t>Switched to 50Hz mode</t>
+  </si>
+  <si>
+    <t>Switched to 4Hz mode</t>
   </si>
 </sst>
 </file>
@@ -3092,7 +3209,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3108,7 +3225,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3406,9 +3523,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA75797-E648-42A0-8371-33110FA3C3B8}">
   <dimension ref="A1:C209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -5726,7 +5845,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
@@ -6029,7 +6148,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="60.140625" style="1" bestFit="1" customWidth="1"/>
@@ -8257,7 +8376,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24" style="1" bestFit="1" customWidth="1"/>
@@ -8560,7 +8679,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -8875,7 +8994,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -11079,11 +11198,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF6F8EA2-3B76-42B1-A29A-AED6DA3FFEF8}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -11595,6 +11716,161 @@
       </c>
       <c r="C46" s="1" t="s">
         <v>214</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>1043</v>
       </c>
     </row>
   </sheetData>
@@ -11608,7 +11884,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="3" width="62.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -13859,7 +14135,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -14161,7 +14437,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
@@ -16202,7 +16478,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="29" bestFit="1" customWidth="1"/>
@@ -16670,7 +16946,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="41.140625" bestFit="1" customWidth="1"/>

</xml_diff>